<commit_message>
fixed anonymous sessions bug
</commit_message>
<xml_diff>
--- a/accounts/static/accounts/textdb.xlsx
+++ b/accounts/static/accounts/textdb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudio\app\Django\accounts\accounts\static\accounts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48DC243-4070-4C94-ACB0-5679D3D792C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED6A66C-41E1-431B-89F5-D42444AC7A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3225" yWindow="2445" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="181">
   <si>
     <t>pt-br</t>
   </si>
@@ -562,6 +562,12 @@
   </si>
   <si>
     <t>txtSearch</t>
+  </si>
+  <si>
+    <t>Anonymous</t>
+  </si>
+  <si>
+    <t>Anônimo</t>
   </si>
 </sst>
 </file>
@@ -900,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:C96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,621 +1039,629 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>19</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>103</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>167</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>53</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>110</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>80</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>59</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>68</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>72</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>82</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>88</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>172</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>92</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>159</v>
+        <v>100</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>162</v>
+        <v>101</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>165</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>168</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>114</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>136</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>170</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>153</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>155</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>157</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>158</v>
       </c>
     </row>

</xml_diff>